<commit_message>
Version final de la RF2
Para la entrega
</commit_message>
<xml_diff>
--- a/Documentos/Planilla de bugs (6+1 Software).xlsx
+++ b/Documentos/Planilla de bugs (6+1 Software).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fede\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\uni\LAB SOFT\TP-MASTER SECURITY SYSTEM\Entregas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215FD981-2735-4E9C-841B-33A7250EB8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D0042-8716-4B35-BD50-4FB29C958827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1928,50 +1928,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="15" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1992,7 +1991,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2290,213 +2289,211 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="19.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="60.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18" style="6" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="31" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="6"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="60.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
+    <col min="10" max="10" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="127.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
+    <row r="4" spans="2:11" ht="108.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>45421</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <v>45421</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="13"/>
-    </row>
-    <row r="5" spans="2:11" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10">
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="2:11" ht="105.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>45421</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="11">
         <v>45421</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="2:11" ht="126" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10">
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="2:11" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>45421</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="11">
         <v>45421</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="2:11" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10">
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="2:11" ht="105.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>45421</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="11">
         <v>45421</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="2:11" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="2:11" ht="95.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>45421</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="11">
         <v>45421</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="2:11" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="2:11" ht="95.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>45421</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="11">
         <v>45421</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>92</v>
       </c>
       <c r="J9" s="5" t="s">
@@ -2504,1498 +2501,1498 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="2:11" ht="127.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10">
+    <row r="10" spans="2:11" ht="108.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>45421</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="11">
         <v>45421</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="2:11" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10">
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="2:11" ht="105.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>45421</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="11">
         <v>45421</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J11" s="13"/>
-    </row>
-    <row r="12" spans="2:11" ht="137.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10">
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="2:11" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>45421</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="11">
         <v>45421</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="2:11" ht="126" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10">
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="2:11" ht="105.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9">
         <v>10</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>45421</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="11">
         <v>45421</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="2:11" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10">
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="2:11" ht="95.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="9">
         <v>11</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>45421</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="11">
         <v>45421</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="2:11" ht="114.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10">
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="2:11" ht="95.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>45421</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="11">
         <v>45421</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="10" t="s">
         <v>92</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10">
+    <row r="16" spans="2:11" ht="85.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="9">
         <v>13</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="11">
         <v>45421</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="11">
         <v>45421</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="10" t="s">
         <v>92</v>
       </c>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:12" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10">
+    <row r="17" spans="2:12" ht="85.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="9">
         <v>14</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="D17" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="11">
         <v>45421</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <v>45421</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>92</v>
       </c>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:12" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
+    <row r="18" spans="2:12" ht="85.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="9">
         <v>15</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="D18" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="11">
         <v>45421</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="11">
         <v>45421</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>92</v>
       </c>
       <c r="J18" s="5"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="2:12" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10">
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="2:12" ht="85.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="9">
         <v>16</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="D19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="11">
         <v>45421</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="11">
         <v>45421</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="10" t="s">
         <v>92</v>
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:12" ht="81" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10">
+    <row r="20" spans="2:12" ht="75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="9">
         <v>17</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="D20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="11">
         <v>45421</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="11">
         <v>45424</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:12" ht="81" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10">
+    <row r="21" spans="2:12" ht="75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="9">
         <v>18</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="11">
         <v>45421</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="11">
         <v>45424</v>
       </c>
-      <c r="I21" s="11"/>
+      <c r="I21" s="10"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="81" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10">
+    <row r="22" spans="2:12" ht="75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="9">
         <v>19</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="12">
+      <c r="D22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="11">
         <v>45421</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="11">
         <v>45424</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:12" ht="81" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10">
+    <row r="23" spans="2:12" ht="75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="9">
         <v>20</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="12">
+      <c r="D23" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="11">
         <v>45421</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="11">
         <v>45424</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:12" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10">
-        <v>21</v>
-      </c>
-      <c r="C24" s="11" t="s">
+    <row r="24" spans="2:12" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="9">
+        <v>21</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="12">
+      <c r="D24" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="11">
         <v>45421</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="11">
         <v>45424</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:12" ht="150" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10">
+    <row r="25" spans="2:12" ht="139.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="9">
         <v>22</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="12">
+      <c r="D25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="11">
         <v>45421</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="11">
         <v>45424</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:12" ht="150" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10">
+    <row r="26" spans="2:12" ht="139.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="9">
         <v>23</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="12">
+      <c r="D26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="11">
         <v>45421</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="11">
         <v>45424</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="2:12" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10">
+    <row r="27" spans="2:12" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="9">
         <v>24</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" s="12">
+      <c r="D27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="11">
         <v>45421</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H27" s="11">
         <v>45424</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:12" ht="150" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10">
+    <row r="28" spans="2:12" ht="139.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="9">
         <v>25</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="12">
+      <c r="D28" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="11">
         <v>45421</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H28" s="11">
         <v>45424</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I28" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J28" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10">
+    <row r="29" spans="2:12" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="9">
         <v>26</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="12">
+      <c r="D29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="11">
         <v>45421</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H29" s="11">
         <v>45424</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:12" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10">
+    <row r="30" spans="2:12" ht="139.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="9">
         <v>27</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="12">
+      <c r="D30" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="11">
         <v>45421</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="12">
+      <c r="H30" s="11">
         <v>45424</v>
       </c>
-      <c r="I30" s="11" t="s">
+      <c r="I30" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="2:12" ht="150" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10">
+    <row r="31" spans="2:12" ht="139.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="9">
         <v>28</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="12">
+      <c r="D31" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="11">
         <v>45421</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="11">
         <v>45424</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="2:12" ht="162.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10">
+    <row r="32" spans="2:12" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="9">
         <v>29</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" s="12">
+      <c r="D32" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="11">
         <v>45421</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="11">
         <v>45424</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="2:10" ht="150" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10">
+    <row r="33" spans="2:10" ht="139.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="9">
         <v>30</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="12">
+      <c r="D33" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="11">
         <v>45421</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G33" s="11" t="s">
+      <c r="G33" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="11">
         <v>45424</v>
       </c>
-      <c r="I33" s="11" t="s">
+      <c r="I33" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J33" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="93.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="10">
+    <row r="34" spans="2:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="9">
         <v>31</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="12">
+      <c r="D34" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="11">
         <v>45422</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11" t="s">
+      <c r="H34" s="10"/>
+      <c r="I34" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="2:10" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="10">
+    <row r="35" spans="2:10" ht="91.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="9">
         <v>32</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E35" s="12">
+      <c r="D35" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="11">
         <v>45422</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11" t="s">
+      <c r="H35" s="10"/>
+      <c r="I35" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="2:10" ht="106.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10">
+    <row r="36" spans="2:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="9">
         <v>33</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="12">
+      <c r="D36" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="11">
         <v>45422</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11" t="s">
+      <c r="H36" s="10"/>
+      <c r="I36" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="2:10" ht="93.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="10">
+    <row r="37" spans="2:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="9">
         <v>34</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="12">
+      <c r="D37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="11">
         <v>45422</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11" t="s">
+      <c r="H37" s="10"/>
+      <c r="I37" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="2:10" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="10">
+    <row r="38" spans="2:10" ht="91.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="9">
         <v>35</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="12">
+      <c r="D38" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="11">
         <v>45422</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11" t="s">
+      <c r="H38" s="10"/>
+      <c r="I38" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10" ht="106.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="10">
+    <row r="39" spans="2:10" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="9">
         <v>36</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="12">
+      <c r="D39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="11">
         <v>45422</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11" t="s">
+      <c r="H39" s="10"/>
+      <c r="I39" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="2:10" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10">
+    <row r="40" spans="2:10" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="9">
         <v>37</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" s="12">
+      <c r="D40" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="11">
         <v>45422</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G40" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11" t="s">
+      <c r="H40" s="10"/>
+      <c r="I40" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="2:10" ht="171" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="10">
+    <row r="41" spans="2:10" ht="169.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="9">
         <v>38</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="12">
+      <c r="D41" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="11">
         <v>45422</v>
       </c>
-      <c r="F41" s="11" t="s">
+      <c r="F41" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G41" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11" t="s">
+      <c r="H41" s="10"/>
+      <c r="I41" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="2:10" ht="172.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="10">
+    <row r="42" spans="2:10" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="9">
         <v>39</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="12">
+      <c r="D42" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="11">
         <v>45422</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11" t="s">
+      <c r="H42" s="10"/>
+      <c r="I42" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="2:10" ht="172.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="10">
+    <row r="43" spans="2:10" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="9">
         <v>40</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D43" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="12">
+      <c r="D43" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="11">
         <v>45422</v>
       </c>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G43" s="11" t="s">
+      <c r="G43" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11" t="s">
+      <c r="H43" s="10"/>
+      <c r="I43" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="10">
+    <row r="44" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="9">
         <v>41</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="12">
+      <c r="D44" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="11">
         <v>45422</v>
       </c>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="G44" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11" t="s">
+      <c r="H44" s="10"/>
+      <c r="I44" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="10">
+    <row r="45" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="9">
         <v>42</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="12">
+      <c r="D45" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="11">
         <v>45422</v>
       </c>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G45" s="11" t="s">
+      <c r="G45" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11" t="s">
+      <c r="H45" s="10"/>
+      <c r="I45" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="10">
+    <row r="46" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="9">
         <v>43</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="12">
+      <c r="D46" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="11">
         <v>45422</v>
       </c>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="G46" s="11" t="s">
+      <c r="G46" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11" t="s">
+      <c r="H46" s="10"/>
+      <c r="I46" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="10">
+    <row r="47" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="9">
         <v>44</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E47" s="12">
+      <c r="D47" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="11">
         <v>45422</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="G47" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11" t="s">
+      <c r="H47" s="10"/>
+      <c r="I47" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="2:10" ht="148.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="10">
+    <row r="48" spans="2:10" ht="136.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="9">
         <v>45</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E48" s="12">
+      <c r="D48" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E48" s="11">
         <v>45422</v>
       </c>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11" t="s">
+      <c r="H48" s="10"/>
+      <c r="I48" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="10">
+    <row r="49" spans="2:10" ht="162.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="9">
         <v>46</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E49" s="12">
+      <c r="D49" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="11">
         <v>45422</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G49" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11" t="s">
+      <c r="H49" s="10"/>
+      <c r="I49" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J49" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="148.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="10">
+    <row r="50" spans="2:10" ht="136.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="9">
         <v>47</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D50" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E50" s="12">
+      <c r="D50" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E50" s="11">
         <v>45422</v>
       </c>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G50" s="11" t="s">
+      <c r="G50" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11" t="s">
+      <c r="H50" s="10"/>
+      <c r="I50" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="10">
+    <row r="51" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="9">
         <v>48</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E51" s="12">
+      <c r="D51" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E51" s="11">
         <v>45422</v>
       </c>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11" t="s">
+      <c r="H51" s="10"/>
+      <c r="I51" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J51" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="148.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="10">
+    <row r="52" spans="2:10" ht="136.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="9">
         <v>49</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D52" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E52" s="12">
+      <c r="D52" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="11">
         <v>45422</v>
       </c>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G52" s="11" t="s">
+      <c r="G52" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11" t="s">
+      <c r="H52" s="10"/>
+      <c r="I52" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="10">
+    <row r="53" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="9">
         <v>50</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D53" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E53" s="12">
+      <c r="D53" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" s="11">
         <v>45422</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G53" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11" t="s">
+      <c r="H53" s="10"/>
+      <c r="I53" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J53" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="2:10" ht="171" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="10">
+    <row r="54" spans="2:10" ht="169.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="9">
         <v>51</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E54" s="12">
+      <c r="D54" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="11">
         <v>45422</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G54" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11" t="s">
+      <c r="H54" s="10"/>
+      <c r="I54" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="2:10" ht="172.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="10">
+    <row r="55" spans="2:10" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="9">
         <v>52</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E55" s="12">
+      <c r="D55" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="11">
         <v>45422</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11" t="s">
+      <c r="H55" s="10"/>
+      <c r="I55" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="2:10" ht="172.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="10">
+    <row r="56" spans="2:10" ht="159.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="9">
         <v>53</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E56" s="12">
+      <c r="D56" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="11">
         <v>45422</v>
       </c>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G56" s="11" t="s">
+      <c r="G56" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11" t="s">
+      <c r="H56" s="10"/>
+      <c r="I56" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="10">
+    <row r="57" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="9">
         <v>54</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" s="12">
+      <c r="D57" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="11">
         <v>45422</v>
       </c>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G57" s="11" t="s">
+      <c r="G57" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11" t="s">
+      <c r="H57" s="10"/>
+      <c r="I57" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="10">
+    <row r="58" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="9">
         <v>55</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D58" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E58" s="12">
+      <c r="D58" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E58" s="11">
         <v>45422</v>
       </c>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G58" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11" t="s">
+      <c r="H58" s="10"/>
+      <c r="I58" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="10">
+    <row r="59" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="9">
         <v>56</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E59" s="12">
+      <c r="D59" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="11">
         <v>45422</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11" t="s">
+      <c r="H59" s="10"/>
+      <c r="I59" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="10">
+    <row r="60" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="9">
         <v>57</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E60" s="12">
+      <c r="D60" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" s="11">
         <v>45422</v>
       </c>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11" t="s">
+      <c r="H60" s="10"/>
+      <c r="I60" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="2:10" ht="148.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="10">
+    <row r="61" spans="2:10" ht="136.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="9">
         <v>58</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D61" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E61" s="12">
+      <c r="D61" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="11">
         <v>45422</v>
       </c>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="G61" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11" t="s">
+      <c r="H61" s="10"/>
+      <c r="I61" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="10">
+    <row r="62" spans="2:10" ht="162.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="9">
         <v>59</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D62" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E62" s="12">
+      <c r="D62" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="11">
         <v>45422</v>
       </c>
-      <c r="F62" s="11" t="s">
+      <c r="F62" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G62" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11" t="s">
+      <c r="H62" s="10"/>
+      <c r="I62" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J62" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="2:10" ht="148.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="10">
+    <row r="63" spans="2:10" ht="136.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="9">
         <v>60</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D63" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E63" s="12">
+      <c r="D63" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" s="11">
         <v>45422</v>
       </c>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G63" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11" t="s">
+      <c r="H63" s="10"/>
+      <c r="I63" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="10">
+    <row r="64" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="9">
         <v>61</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D64" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E64" s="12">
+      <c r="D64" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="11">
         <v>45422</v>
       </c>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G64" s="11" t="s">
+      <c r="G64" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11" t="s">
+      <c r="H64" s="10"/>
+      <c r="I64" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J64" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="2:10" ht="148.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="10">
+    <row r="65" spans="2:10" ht="136.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="9">
         <v>62</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D65" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E65" s="12">
+      <c r="D65" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" s="11">
         <v>45422</v>
       </c>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G65" s="11" t="s">
+      <c r="G65" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11" t="s">
+      <c r="H65" s="10"/>
+      <c r="I65" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="2:10" ht="161.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="10">
+    <row r="66" spans="2:10" ht="149.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="9">
         <v>63</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D66" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E66" s="12">
+      <c r="D66" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" s="11">
         <v>45422</v>
       </c>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="G66" s="11" t="s">
+      <c r="G66" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11" t="s">
+      <c r="H66" s="10"/>
+      <c r="I66" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J66" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="2"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -4006,7 +4003,7 @@
       <c r="I67" s="3"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="2"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -4017,7 +4014,7 @@
       <c r="I68" s="3"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B69" s="2"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -4028,7 +4025,7 @@
       <c r="I69" s="3"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" s="2"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -4039,7 +4036,7 @@
       <c r="I70" s="3"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" s="2"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -4050,7 +4047,7 @@
       <c r="I71" s="3"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B72" s="2"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -4061,7 +4058,7 @@
       <c r="I72" s="3"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B73" s="2"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -4072,7 +4069,7 @@
       <c r="I73" s="3"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="2"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -4083,7 +4080,7 @@
       <c r="I74" s="3"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B75" s="2"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -4094,7 +4091,7 @@
       <c r="I75" s="3"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B76" s="2"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -4105,7 +4102,7 @@
       <c r="I76" s="3"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="2"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -4116,7 +4113,7 @@
       <c r="I77" s="3"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B78" s="2"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -4127,7 +4124,7 @@
       <c r="I78" s="3"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="2"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -4138,7 +4135,7 @@
       <c r="I79" s="3"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="2"/>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -4149,7 +4146,7 @@
       <c r="I80" s="3"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B81" s="2"/>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -4160,7 +4157,7 @@
       <c r="I81" s="3"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B82" s="2"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -4171,7 +4168,7 @@
       <c r="I82" s="3"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B83" s="2"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -4182,7 +4179,7 @@
       <c r="I83" s="3"/>
       <c r="J83" s="5"/>
     </row>
-    <row r="84" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B84" s="2"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -4193,7 +4190,7 @@
       <c r="I84" s="3"/>
       <c r="J84" s="5"/>
     </row>
-    <row r="85" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B85" s="2"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -4204,7 +4201,7 @@
       <c r="I85" s="3"/>
       <c r="J85" s="5"/>
     </row>
-    <row r="86" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B86" s="2"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -4215,7 +4212,7 @@
       <c r="I86" s="3"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B87" s="2"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -4226,7 +4223,7 @@
       <c r="I87" s="3"/>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B88" s="2"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -4237,7 +4234,7 @@
       <c r="I88" s="3"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B89" s="2"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -4248,7 +4245,7 @@
       <c r="I89" s="3"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B90" s="2"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -4259,7 +4256,7 @@
       <c r="I90" s="3"/>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B91" s="2"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -4270,7 +4267,7 @@
       <c r="I91" s="3"/>
       <c r="J91" s="5"/>
     </row>
-    <row r="92" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B92" s="2"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
@@ -4281,7 +4278,7 @@
       <c r="I92" s="3"/>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="2"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -4292,7 +4289,7 @@
       <c r="I93" s="3"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="2"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
@@ -4303,7 +4300,7 @@
       <c r="I94" s="3"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B95" s="2"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
@@ -4314,7 +4311,7 @@
       <c r="I95" s="3"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B96" s="2"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
@@ -4325,7 +4322,7 @@
       <c r="I96" s="3"/>
       <c r="J96" s="5"/>
     </row>
-    <row r="97" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B97" s="2"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
@@ -4336,7 +4333,7 @@
       <c r="I97" s="3"/>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B98" s="2"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -4347,7 +4344,7 @@
       <c r="I98" s="3"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B99" s="2"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -4358,7 +4355,7 @@
       <c r="I99" s="3"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="2"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -4369,7 +4366,7 @@
       <c r="I100" s="3"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B101" s="2"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
@@ -4380,7 +4377,7 @@
       <c r="I101" s="3"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B102" s="2"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
@@ -4391,7 +4388,7 @@
       <c r="I102" s="3"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B103" s="2"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -4402,7 +4399,7 @@
       <c r="I103" s="3"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B104" s="2"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
@@ -4413,7 +4410,7 @@
       <c r="I104" s="3"/>
       <c r="J104" s="5"/>
     </row>
-    <row r="105" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="2"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
@@ -4424,7 +4421,7 @@
       <c r="I105" s="3"/>
       <c r="J105" s="5"/>
     </row>
-    <row r="106" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="2"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -4435,7 +4432,7 @@
       <c r="I106" s="3"/>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="2"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -4446,7 +4443,7 @@
       <c r="I107" s="3"/>
       <c r="J107" s="5"/>
     </row>
-    <row r="108" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="2"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
@@ -4457,7 +4454,7 @@
       <c r="I108" s="3"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B109" s="2"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
@@ -4468,7 +4465,7 @@
       <c r="I109" s="3"/>
       <c r="J109" s="5"/>
     </row>
-    <row r="110" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B110" s="2"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -4479,7 +4476,7 @@
       <c r="I110" s="3"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B111" s="2"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -4490,7 +4487,7 @@
       <c r="I111" s="3"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="2"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
@@ -4501,7 +4498,7 @@
       <c r="I112" s="3"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="2"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
@@ -4512,7 +4509,7 @@
       <c r="I113" s="3"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="2"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
@@ -4523,7 +4520,7 @@
       <c r="I114" s="3"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="2"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -4534,7 +4531,7 @@
       <c r="I115" s="3"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="2"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
@@ -4545,7 +4542,7 @@
       <c r="I116" s="3"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="2"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -4556,7 +4553,7 @@
       <c r="I117" s="3"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B118" s="2"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
@@ -4567,7 +4564,7 @@
       <c r="I118" s="3"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="2"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
@@ -4578,7 +4575,7 @@
       <c r="I119" s="3"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B120" s="2"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
@@ -4589,7 +4586,7 @@
       <c r="I120" s="3"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B121" s="2"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
@@ -4600,7 +4597,7 @@
       <c r="I121" s="3"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B122" s="2"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
@@ -4611,7 +4608,7 @@
       <c r="I122" s="3"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B123" s="2"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
@@ -4622,7 +4619,7 @@
       <c r="I123" s="3"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B124" s="2"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -4633,7 +4630,7 @@
       <c r="I124" s="3"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="2"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
@@ -4644,7 +4641,7 @@
       <c r="I125" s="3"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="2"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
@@ -4655,7 +4652,7 @@
       <c r="I126" s="3"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B127" s="2"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
@@ -4666,7 +4663,7 @@
       <c r="I127" s="3"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B128" s="2"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
@@ -4677,7 +4674,7 @@
       <c r="I128" s="3"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B129" s="2"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
@@ -4688,7 +4685,7 @@
       <c r="I129" s="3"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B130" s="2"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
@@ -4699,7 +4696,7 @@
       <c r="I130" s="3"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B131" s="2"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
@@ -4710,7 +4707,7 @@
       <c r="I131" s="3"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B132" s="2"/>
       <c r="C132" s="3"/>
       <c r="D132" s="3"/>
@@ -4721,7 +4718,7 @@
       <c r="I132" s="3"/>
       <c r="J132" s="5"/>
     </row>
-    <row r="133" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="2"/>
       <c r="C133" s="3"/>
       <c r="D133" s="3"/>
@@ -4732,7 +4729,7 @@
       <c r="I133" s="3"/>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B134" s="2"/>
       <c r="C134" s="3"/>
       <c r="D134" s="3"/>
@@ -4743,7 +4740,7 @@
       <c r="I134" s="3"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="2"/>
       <c r="C135" s="3"/>
       <c r="D135" s="3"/>
@@ -4754,7 +4751,7 @@
       <c r="I135" s="3"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B136" s="2"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
@@ -4765,7 +4762,7 @@
       <c r="I136" s="3"/>
       <c r="J136" s="5"/>
     </row>
-    <row r="137" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="2"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
@@ -4776,7 +4773,7 @@
       <c r="I137" s="3"/>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B138" s="2"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
@@ -4787,7 +4784,7 @@
       <c r="I138" s="3"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B139" s="2"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
@@ -4798,7 +4795,7 @@
       <c r="I139" s="3"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B140" s="2"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
@@ -4809,7 +4806,7 @@
       <c r="I140" s="3"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B141" s="2"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
@@ -4820,7 +4817,7 @@
       <c r="I141" s="3"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="2"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
@@ -4831,7 +4828,7 @@
       <c r="I142" s="3"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="2"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
@@ -4842,7 +4839,7 @@
       <c r="I143" s="3"/>
       <c r="J143" s="5"/>
     </row>
-    <row r="144" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B144" s="2"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -4853,7 +4850,7 @@
       <c r="I144" s="3"/>
       <c r="J144" s="5"/>
     </row>
-    <row r="145" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B145" s="2"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
@@ -4864,7 +4861,7 @@
       <c r="I145" s="3"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B146" s="2"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
@@ -4875,7 +4872,7 @@
       <c r="I146" s="3"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B147" s="2"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
@@ -4886,7 +4883,7 @@
       <c r="I147" s="3"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B148" s="2"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
@@ -4897,7 +4894,7 @@
       <c r="I148" s="3"/>
       <c r="J148" s="5"/>
     </row>
-    <row r="149" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="2"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
@@ -4908,7 +4905,7 @@
       <c r="I149" s="3"/>
       <c r="J149" s="5"/>
     </row>
-    <row r="150" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="2"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
@@ -4919,7 +4916,7 @@
       <c r="I150" s="3"/>
       <c r="J150" s="5"/>
     </row>
-    <row r="151" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="2"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>

</xml_diff>